<commit_message>
finished transforming DonateNYC data to xlsx sheet
</commit_message>
<xml_diff>
--- a/data/DonateNYC.xlsx
+++ b/data/DonateNYC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -441,6 +441,78 @@
   </si>
   <si>
     <t xml:space="preserve">148-15 Archer Avenue </t>
+  </si>
+  <si>
+    <t>Lower East Side Ecology Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">469 President Street </t>
+  </si>
+  <si>
+    <t>(718) 858-8777</t>
+  </si>
+  <si>
+    <t>http://www.lesecologycenter.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Quincy Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 Second Avenue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">112 Fourth Avenue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">44 West 8th Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 West 14th Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">120 West 14th Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">220 East 23rd Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">208 E 23rd Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">208 Eighth Avenue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">103 West 25th Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 East 37th St. 5th Floor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">520 8th Avenue 10th Floor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1158 Flatbush Avenue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">555 West 42 Street </t>
+  </si>
+  <si>
+    <t xml:space="preserve">536 W. 46th St. </t>
+  </si>
+  <si>
+    <t>Life of Hope, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1886 Nostrand Avenue 1FL </t>
+  </si>
+  <si>
+    <t>(718) 362-3162</t>
+  </si>
+  <si>
+    <t>http://www.lohnyc.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6822 Third Avenue </t>
   </si>
 </sst>
 </file>
@@ -496,8 +568,378 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="391">
+  <cellStyleXfs count="761">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -893,7 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="391">
+  <cellStyles count="761">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1089,6 +1531,191 @@
     <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1284,6 +1911,191 @@
     <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1559,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4056,6 +4868,980 @@
         <v>31</v>
       </c>
     </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88">
+        <v>11201</v>
+      </c>
+      <c r="F88" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89">
+        <v>11217</v>
+      </c>
+      <c r="F89" t="s">
+        <v>26</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E90">
+        <v>11217</v>
+      </c>
+      <c r="F90" t="s">
+        <v>72</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" t="s">
+        <v>139</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91">
+        <v>11215</v>
+      </c>
+      <c r="F91" t="s">
+        <v>140</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92">
+        <v>11238</v>
+      </c>
+      <c r="F92" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93">
+        <v>11249</v>
+      </c>
+      <c r="F93" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>43</v>
+      </c>
+      <c r="B94" t="s">
+        <v>47</v>
+      </c>
+      <c r="C94" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94">
+        <v>10009</v>
+      </c>
+      <c r="F94" t="s">
+        <v>45</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>43</v>
+      </c>
+      <c r="B95" t="s">
+        <v>143</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95">
+        <v>10003</v>
+      </c>
+      <c r="F95" t="s">
+        <v>45</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" t="s">
+        <v>144</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96">
+        <v>10003</v>
+      </c>
+      <c r="F96" t="s">
+        <v>26</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>65</v>
+      </c>
+      <c r="B97" t="s">
+        <v>66</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97">
+        <v>11206</v>
+      </c>
+      <c r="F97" t="s">
+        <v>67</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98">
+        <v>10011</v>
+      </c>
+      <c r="F98" t="s">
+        <v>30</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" t="s">
+        <v>146</v>
+      </c>
+      <c r="C99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99">
+        <v>10011</v>
+      </c>
+      <c r="F99" t="s">
+        <v>30</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" t="s">
+        <v>147</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100">
+        <v>10011</v>
+      </c>
+      <c r="F100" t="s">
+        <v>26</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>28</v>
+      </c>
+      <c r="B101" t="s">
+        <v>148</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101">
+        <v>10010</v>
+      </c>
+      <c r="F101" t="s">
+        <v>30</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>24</v>
+      </c>
+      <c r="B102" t="s">
+        <v>149</v>
+      </c>
+      <c r="C102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102">
+        <v>10010</v>
+      </c>
+      <c r="F102" t="s">
+        <v>26</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>24</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103">
+        <v>11222</v>
+      </c>
+      <c r="F103" t="s">
+        <v>26</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104" t="s">
+        <v>118</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104">
+        <v>11213</v>
+      </c>
+      <c r="F104" t="s">
+        <v>119</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" t="s">
+        <v>129</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105">
+        <v>11221</v>
+      </c>
+      <c r="F105" t="s">
+        <v>130</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>24</v>
+      </c>
+      <c r="B106" t="s">
+        <v>150</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106">
+        <v>10011</v>
+      </c>
+      <c r="F106" t="s">
+        <v>26</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="H106" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" t="s">
+        <v>151</v>
+      </c>
+      <c r="C107" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107">
+        <v>10001</v>
+      </c>
+      <c r="F107" t="s">
+        <v>30</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>83</v>
+      </c>
+      <c r="B108" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108">
+        <v>10001</v>
+      </c>
+      <c r="F108" t="s">
+        <v>18</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="H108" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>33</v>
+      </c>
+      <c r="B109" t="s">
+        <v>152</v>
+      </c>
+      <c r="C109" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109">
+        <v>10016</v>
+      </c>
+      <c r="F109" t="s">
+        <v>35</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>97</v>
+      </c>
+      <c r="B110" t="s">
+        <v>98</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110">
+        <v>11233</v>
+      </c>
+      <c r="F110" t="s">
+        <v>99</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="H110" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>153</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111">
+        <v>10018</v>
+      </c>
+      <c r="F111" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="H111" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" t="s">
+        <v>49</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112">
+        <v>11101</v>
+      </c>
+      <c r="F112" t="s">
+        <v>51</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>93</v>
+      </c>
+      <c r="B113" t="s">
+        <v>94</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E113">
+        <v>11385</v>
+      </c>
+      <c r="F113" t="s">
+        <v>95</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114" t="s">
+        <v>57</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114">
+        <v>11101</v>
+      </c>
+      <c r="F114" t="s">
+        <v>30</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="H114" t="s">
+        <v>14</v>
+      </c>
+      <c r="I114" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>65</v>
+      </c>
+      <c r="B115" t="s">
+        <v>154</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115">
+        <v>11226</v>
+      </c>
+      <c r="F115" t="s">
+        <v>67</v>
+      </c>
+      <c r="G115">
+        <v>1</v>
+      </c>
+      <c r="H115" t="s">
+        <v>14</v>
+      </c>
+      <c r="I115" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116" t="s">
+        <v>155</v>
+      </c>
+      <c r="C116" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116">
+        <v>10036</v>
+      </c>
+      <c r="F116" t="s">
+        <v>22</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116" t="s">
+        <v>14</v>
+      </c>
+      <c r="I116" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>24</v>
+      </c>
+      <c r="B117" t="s">
+        <v>156</v>
+      </c>
+      <c r="C117" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" t="s">
+        <v>12</v>
+      </c>
+      <c r="E117">
+        <v>10036</v>
+      </c>
+      <c r="F117" t="s">
+        <v>26</v>
+      </c>
+      <c r="G117">
+        <v>1</v>
+      </c>
+      <c r="H117" t="s">
+        <v>14</v>
+      </c>
+      <c r="I117" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>157</v>
+      </c>
+      <c r="B118" t="s">
+        <v>158</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118">
+        <v>11226</v>
+      </c>
+      <c r="F118" t="s">
+        <v>159</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
+      </c>
+      <c r="H118" t="s">
+        <v>14</v>
+      </c>
+      <c r="I118" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>109</v>
+      </c>
+      <c r="B119" t="s">
+        <v>110</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119">
+        <v>11230</v>
+      </c>
+      <c r="F119" t="s">
+        <v>111</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119" t="s">
+        <v>14</v>
+      </c>
+      <c r="I119" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>24</v>
+      </c>
+      <c r="B120" t="s">
+        <v>161</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120">
+        <v>11220</v>
+      </c>
+      <c r="F120" t="s">
+        <v>26</v>
+      </c>
+      <c r="G120">
+        <v>1</v>
+      </c>
+      <c r="H120" t="s">
+        <v>14</v>
+      </c>
+      <c r="I120" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>43</v>
+      </c>
+      <c r="B121" t="s">
+        <v>136</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121">
+        <v>11207</v>
+      </c>
+      <c r="F121" t="s">
+        <v>45</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>